<commit_message>
added multiple benchmarks (DFT, SFT)
</commit_message>
<xml_diff>
--- a/models/ctmc/epidemic/parameters.xlsx
+++ b/models/ctmc/epidemic/parameters.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
   <si>
     <t>name</t>
   </si>
@@ -49,123 +49,63 @@
     <t>label</t>
   </si>
   <si>
-    <t>P=? [ (popI&gt;0) U[100,105] (popI=0) ]</t>
-  </si>
-  <si>
     <t>P=? [ (popI&gt;0) U[100,110] (popI=0) ]</t>
   </si>
   <si>
-    <t>P=? [ (popI&gt;0) U[100,115] (popI=0) ]</t>
-  </si>
-  <si>
     <t>P=? [ (popI&gt;0) U[100,120] (popI=0) ]</t>
   </si>
   <si>
-    <t>P=? [ (popI&gt;0) U[100,125] (popI=0) ]</t>
-  </si>
-  <si>
     <t>P=? [ (popI&gt;0) U[100,130] (popI=0) ]</t>
   </si>
   <si>
-    <t>P=? [ (popI&gt;0) U[100,135] (popI=0) ]</t>
-  </si>
-  <si>
     <t>P=? [ (popI&gt;0) U[100,140] (popI=0) ]</t>
   </si>
   <si>
-    <t>P=? [ (popI&gt;0) U[100,145] (popI=0) ]</t>
-  </si>
-  <si>
     <t>P=? [ (popI&gt;0) U[100,150] (popI=0) ]</t>
   </si>
   <si>
-    <t>P=? [ (popI&gt;0) U[100,155] (popI=0) ]</t>
-  </si>
-  <si>
     <t>P=? [ (popI&gt;0) U[100,160] (popI=0) ]</t>
   </si>
   <si>
-    <t>P=? [ (popI&gt;0) U[100,165] (popI=0) ]</t>
-  </si>
-  <si>
     <t>P=? [ (popI&gt;0) U[100,170] (popI=0) ]</t>
   </si>
   <si>
-    <t>P=? [ (popI&gt;0) U[100,175] (popI=0) ]</t>
-  </si>
-  <si>
     <t>P=? [ (popI&gt;0) U[100,180] (popI=0) ]</t>
   </si>
   <si>
-    <t>P=? [ (popI&gt;0) U[100,185] (popI=0) ]</t>
-  </si>
-  <si>
     <t>P=? [ (popI&gt;0) U[100,190] (popI=0) ]</t>
   </si>
   <si>
-    <t>P=? [ (popI&gt;0) U[100,195] (popI=0) ]</t>
-  </si>
-  <si>
     <t>P=? [ (popI&gt;0) U[100,200] (popI=0) ]</t>
   </si>
   <si>
-    <t>Rel T=105</t>
-  </si>
-  <si>
     <t>Rel T=110</t>
   </si>
   <si>
-    <t>Rel T=115</t>
-  </si>
-  <si>
     <t>Rel T=120</t>
   </si>
   <si>
-    <t>Rel T=125</t>
-  </si>
-  <si>
     <t>Rel T=130</t>
   </si>
   <si>
-    <t>Rel T=135</t>
-  </si>
-  <si>
     <t>Rel T=140</t>
   </si>
   <si>
-    <t>Rel T=145</t>
-  </si>
-  <si>
     <t>Rel T=150</t>
   </si>
   <si>
-    <t>Rel T=155</t>
-  </si>
-  <si>
     <t>Rel T=160</t>
   </si>
   <si>
-    <t>Rel T=165</t>
-  </si>
-  <si>
     <t>Rel T=170</t>
   </si>
   <si>
-    <t>Rel T=175</t>
-  </si>
-  <si>
     <t>Rel T=180</t>
   </si>
   <si>
-    <t>Rel T=185</t>
-  </si>
-  <si>
     <t>Rel T=190</t>
   </si>
   <si>
-    <t>Rel T=195</t>
-  </si>
-  <si>
     <t>Rel T=200</t>
   </si>
   <si>
@@ -173,6 +113,246 @@
   </si>
   <si>
     <t>enabled</t>
+  </si>
+  <si>
+    <t>Rel T=102</t>
+  </si>
+  <si>
+    <t>Rel T=104</t>
+  </si>
+  <si>
+    <t>Rel T=106</t>
+  </si>
+  <si>
+    <t>Rel T=108</t>
+  </si>
+  <si>
+    <t>Rel T=112</t>
+  </si>
+  <si>
+    <t>Rel T=114</t>
+  </si>
+  <si>
+    <t>Rel T=116</t>
+  </si>
+  <si>
+    <t>Rel T=118</t>
+  </si>
+  <si>
+    <t>Rel T=122</t>
+  </si>
+  <si>
+    <t>Rel T=124</t>
+  </si>
+  <si>
+    <t>Rel T=126</t>
+  </si>
+  <si>
+    <t>Rel T=128</t>
+  </si>
+  <si>
+    <t>Rel T=132</t>
+  </si>
+  <si>
+    <t>Rel T=134</t>
+  </si>
+  <si>
+    <t>Rel T=136</t>
+  </si>
+  <si>
+    <t>Rel T=138</t>
+  </si>
+  <si>
+    <t>Rel T=142</t>
+  </si>
+  <si>
+    <t>Rel T=144</t>
+  </si>
+  <si>
+    <t>Rel T=146</t>
+  </si>
+  <si>
+    <t>Rel T=148</t>
+  </si>
+  <si>
+    <t>Rel T=152</t>
+  </si>
+  <si>
+    <t>Rel T=154</t>
+  </si>
+  <si>
+    <t>Rel T=156</t>
+  </si>
+  <si>
+    <t>Rel T=158</t>
+  </si>
+  <si>
+    <t>Rel T=162</t>
+  </si>
+  <si>
+    <t>Rel T=164</t>
+  </si>
+  <si>
+    <t>Rel T=166</t>
+  </si>
+  <si>
+    <t>Rel T=168</t>
+  </si>
+  <si>
+    <t>Rel T=172</t>
+  </si>
+  <si>
+    <t>Rel T=174</t>
+  </si>
+  <si>
+    <t>Rel T=176</t>
+  </si>
+  <si>
+    <t>Rel T=178</t>
+  </si>
+  <si>
+    <t>Rel T=182</t>
+  </si>
+  <si>
+    <t>Rel T=184</t>
+  </si>
+  <si>
+    <t>Rel T=186</t>
+  </si>
+  <si>
+    <t>Rel T=188</t>
+  </si>
+  <si>
+    <t>Rel T=192</t>
+  </si>
+  <si>
+    <t>Rel T=194</t>
+  </si>
+  <si>
+    <t>Rel T=196</t>
+  </si>
+  <si>
+    <t>Rel T=198</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,102] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,104] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,106] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,108] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,112] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,114] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,116] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,118] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,122] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,124] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,126] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,128] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,132] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,134] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,136] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,138] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,142] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,144] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,146] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,148] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,192] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,194] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,196] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,198] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,152] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,154] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,156] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,158] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,162] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,164] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,166] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,168] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,172] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,174] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,176] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,178] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,182] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,184] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,186] (popI=0) ]</t>
+  </si>
+  <si>
+    <t>P=? [ (popI&gt;0) U[100,188] (popI=0) ]</t>
   </si>
 </sst>
 </file>
@@ -547,10 +727,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,21 +747,21 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="C2">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -589,13 +769,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="C3">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -603,13 +783,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="C4">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -617,13 +797,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="C5">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -631,13 +811,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -645,13 +825,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C7">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
@@ -659,13 +839,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="C8">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
@@ -673,13 +853,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="C9">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
@@ -687,13 +867,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="C10">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -701,13 +881,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -718,10 +898,10 @@
         <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="C12">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -732,10 +912,10 @@
         <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C13">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -746,10 +926,10 @@
         <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="C14">
-        <v>165</v>
+        <v>126</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -760,10 +940,10 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C15">
-        <v>170</v>
+        <v>128</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
@@ -771,13 +951,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>175</v>
+        <v>130</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
@@ -785,13 +965,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C17">
-        <v>180</v>
+        <v>132</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -799,13 +979,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="C18">
-        <v>185</v>
+        <v>134</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
@@ -813,13 +993,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="C19">
-        <v>190</v>
+        <v>136</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
@@ -827,13 +1007,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="C20">
-        <v>195</v>
+        <v>138</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
@@ -841,15 +1021,435 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>140</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22">
+        <v>142</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>48</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23">
+        <v>144</v>
+      </c>
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24">
+        <v>146</v>
+      </c>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25">
+        <v>148</v>
+      </c>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26">
+        <v>150</v>
+      </c>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27">
+        <v>152</v>
+      </c>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28">
+        <v>154</v>
+      </c>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29">
+        <v>156</v>
+      </c>
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30">
+        <v>158</v>
+      </c>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>160</v>
+      </c>
+      <c r="D31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32">
+        <v>162</v>
+      </c>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33">
+        <v>164</v>
+      </c>
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34">
+        <v>166</v>
+      </c>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35">
+        <v>168</v>
+      </c>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36">
+        <v>170</v>
+      </c>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37">
+        <v>172</v>
+      </c>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38">
+        <v>174</v>
+      </c>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39">
+        <v>176</v>
+      </c>
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40">
+        <v>178</v>
+      </c>
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41">
+        <v>180</v>
+      </c>
+      <c r="D41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42">
+        <v>182</v>
+      </c>
+      <c r="D42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43">
+        <v>184</v>
+      </c>
+      <c r="D43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44">
+        <v>186</v>
+      </c>
+      <c r="D44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45">
+        <v>188</v>
+      </c>
+      <c r="D45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46">
+        <v>190</v>
+      </c>
+      <c r="D46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47">
+        <v>192</v>
+      </c>
+      <c r="D47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48">
+        <v>194</v>
+      </c>
+      <c r="D48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49">
+        <v>196</v>
+      </c>
+      <c r="D49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50">
+        <v>198</v>
+      </c>
+      <c r="D50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>28</v>
       </c>
-      <c r="C21">
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51">
         <v>200</v>
       </c>
-      <c r="D21" t="b">
+      <c r="D51" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed epidemic (SIR) models from Excel to CSV input format
</commit_message>
<xml_diff>
--- a/models/ctmc/epidemic/parameters.xlsx
+++ b/models/ctmc/epidemic/parameters.xlsx
@@ -1,18 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85F3649-E267-461F-AA11-F009FF6C1F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -45,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -79,7 +90,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -356,11 +367,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>